<commit_message>
v.0.4.0 Database being POPULATED
</commit_message>
<xml_diff>
--- a/assets/DisneyPlus.xlsx
+++ b/assets/DisneyPlus.xlsx
@@ -15904,7 +15904,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15915,6 +15915,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -15948,19 +15954,19 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -15970,7 +15976,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -16353,7 +16359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -16389,7 +16395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -16425,7 +16431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -16463,7 +16469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -16499,7 +16505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -16531,7 +16537,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -16569,7 +16575,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -16603,7 +16609,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -16639,7 +16645,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -16675,7 +16681,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -16713,7 +16719,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -16749,7 +16755,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -16781,7 +16787,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -16819,7 +16825,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>14</v>
       </c>

</xml_diff>